<commit_message>
fixed indices for tables
</commit_message>
<xml_diff>
--- a/wrangled/AEDC.xlsx
+++ b/wrangled/AEDC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DRIVE\Uni\2021\COMP20008 Elements of Data Processing\ass2\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DRIVE\Uni\2021\COMP20008 Elements of Data Processing\ass2\wrangled\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31ED69AD-0289-4CC6-AF6A-ED6320905ED6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B05540-4804-466B-B5D0-ABBD9A12CEBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10110" yWindow="1260" windowWidth="19830" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14370" yWindow="2025" windowWidth="19830" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="91">
   <si>
     <t>LGA</t>
   </si>
@@ -298,9 +298,6 @@
   </si>
   <si>
     <t>Yarriambiack (S)</t>
-  </si>
-  <si>
-    <t>Unincorporated Vic</t>
   </si>
 </sst>
 </file>
@@ -601,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -3422,33 +3419,15 @@
       </c>
     </row>
     <row r="81" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A81" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G81" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H81" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="I81" s="5" t="s">
-        <v>72</v>
-      </c>
+      <c r="A81" s="4"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="5"/>
       <c r="J81" s="5" t="s">
         <v>72</v>
       </c>

</xml_diff>